<commit_message>
parser seems to be finished
</commit_message>
<xml_diff>
--- a/src/main/resources/blacklist.xlsx
+++ b/src/main/resources/blacklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarekjal\IdeaProjects\excel\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaroslaw.jaloszynski\IdeaProjects\excel\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABAB030-BE0C-4FDB-923F-4CB94B47B674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="32385" yWindow="6690" windowWidth="25305" windowHeight="10965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vessels blacklist" sheetId="1" r:id="rId1"/>
@@ -20,21 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="80">
   <si>
     <t>Identifier type</t>
   </si>
@@ -259,12 +251,27 @@
   </si>
   <si>
     <t>28454561111</t>
+  </si>
+  <si>
+    <t>32.01.2022</t>
+  </si>
+  <si>
+    <t>66.13.4567</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>valid reason</t>
+  </si>
+  <si>
+    <t>hhh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -659,25 +666,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -685,7 +692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
@@ -693,7 +700,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -701,7 +708,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -724,24 +731,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="2">
-        <v>44566</v>
+      <c r="C8" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -750,11 +757,13 @@
         <v>44566</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -765,11 +774,15 @@
         <v>44566</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -784,22 +797,22 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="1">
         <v>12345</v>
       </c>
-      <c r="C12" s="2">
-        <v>44565</v>
+      <c r="C12" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -814,13 +827,11 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
-        <v>82713</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="2">
         <v>44565</v>
       </c>
@@ -829,7 +840,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -844,7 +855,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -866,25 +877,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -892,7 +903,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
@@ -900,7 +911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -908,7 +919,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -931,7 +942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -946,7 +957,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -961,7 +972,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -976,7 +987,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -991,7 +1002,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1006,7 +1017,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1021,7 +1032,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1036,7 +1047,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -1051,7 +1062,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1066,7 +1077,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1081,7 +1092,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1098,7 +1109,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1115,7 +1126,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1132,7 +1143,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -1149,7 +1160,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1164,7 +1175,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1179,7 +1190,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1194,7 +1205,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1209,7 +1220,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1224,7 +1235,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1239,7 +1250,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -1254,7 +1265,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1269,7 +1280,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
@@ -1284,7 +1295,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -1299,7 +1310,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
@@ -1314,7 +1325,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>24</v>
       </c>
@@ -1329,7 +1340,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>24</v>
       </c>
@@ -1344,7 +1355,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>24</v>
       </c>
@@ -1359,7 +1370,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>24</v>
       </c>
@@ -1374,7 +1385,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>24</v>
       </c>
@@ -1389,7 +1400,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>24</v>
       </c>
@@ -1404,7 +1415,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>24</v>
       </c>
@@ -1419,7 +1430,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>24</v>
       </c>
@@ -1434,7 +1445,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>24</v>
       </c>
@@ -1449,7 +1460,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>24</v>
       </c>
@@ -1464,7 +1475,7 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>24</v>
       </c>
@@ -1479,7 +1490,7 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>24</v>
       </c>
@@ -1494,7 +1505,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>24</v>
       </c>
@@ -1509,7 +1520,7 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
@@ -1524,7 +1535,7 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>24</v>
       </c>
@@ -1539,7 +1550,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>24</v>
       </c>
@@ -1554,7 +1565,7 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>24</v>
       </c>
@@ -1569,7 +1580,7 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>24</v>
       </c>
@@ -1584,7 +1595,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>24</v>
       </c>
@@ -1599,7 +1610,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>24</v>
       </c>
@@ -1614,7 +1625,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>24</v>
       </c>
@@ -1629,7 +1640,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>24</v>
       </c>
@@ -1644,7 +1655,7 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>24</v>
       </c>
@@ -1659,7 +1670,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>24</v>
       </c>
@@ -1674,7 +1685,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>24</v>
       </c>
@@ -1689,7 +1700,7 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>24</v>
       </c>
@@ -1704,7 +1715,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>24</v>
       </c>
@@ -1719,7 +1730,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>24</v>
       </c>
@@ -1734,7 +1745,7 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>24</v>
       </c>
@@ -1749,7 +1760,7 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>24</v>
       </c>
@@ -1764,7 +1775,7 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>24</v>
       </c>
@@ -1779,7 +1790,7 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>24</v>
       </c>
@@ -1794,7 +1805,7 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>24</v>
       </c>
@@ -1809,7 +1820,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>24</v>
       </c>
@@ -1824,7 +1835,7 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>24</v>
       </c>
@@ -1839,7 +1850,7 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>24</v>
       </c>
@@ -1854,7 +1865,7 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>24</v>
       </c>
@@ -1869,7 +1880,7 @@
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>24</v>
       </c>
@@ -1884,7 +1895,7 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>24</v>
       </c>
@@ -1899,7 +1910,7 @@
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>24</v>
       </c>
@@ -1914,7 +1925,7 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>24</v>
       </c>
@@ -1929,7 +1940,7 @@
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>24</v>
       </c>
@@ -1944,7 +1955,7 @@
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>24</v>
       </c>
@@ -1959,7 +1970,7 @@
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>24</v>
       </c>
@@ -1974,7 +1985,7 @@
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>24</v>
       </c>
@@ -1989,7 +2000,7 @@
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>24</v>
       </c>
@@ -2004,7 +2015,7 @@
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>24</v>
       </c>
@@ -2019,7 +2030,7 @@
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>24</v>
       </c>
@@ -2034,7 +2045,7 @@
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>24</v>
       </c>
@@ -2049,7 +2060,7 @@
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>24</v>
       </c>
@@ -2064,7 +2075,7 @@
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>24</v>
       </c>
@@ -2079,7 +2090,7 @@
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>24</v>
       </c>
@@ -2094,7 +2105,7 @@
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>24</v>
       </c>
@@ -2109,7 +2120,7 @@
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>24</v>
       </c>
@@ -2124,7 +2135,7 @@
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>24</v>
       </c>
@@ -2139,7 +2150,7 @@
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>24</v>
       </c>
@@ -2154,7 +2165,7 @@
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>24</v>
       </c>
@@ -2169,7 +2180,7 @@
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>24</v>
       </c>
@@ -2184,7 +2195,7 @@
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>24</v>
       </c>
@@ -2199,7 +2210,7 @@
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>24</v>
       </c>
@@ -2214,7 +2225,7 @@
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>24</v>
       </c>
@@ -2229,7 +2240,7 @@
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>24</v>
       </c>
@@ -2244,7 +2255,7 @@
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>24</v>
       </c>
@@ -2259,7 +2270,7 @@
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>24</v>
       </c>
@@ -2274,7 +2285,7 @@
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>24</v>
       </c>
@@ -2289,7 +2300,7 @@
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>24</v>
       </c>
@@ -2304,7 +2315,7 @@
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>24</v>
       </c>
@@ -2319,7 +2330,7 @@
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>24</v>
       </c>
@@ -2334,7 +2345,7 @@
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>24</v>
       </c>
@@ -2349,7 +2360,7 @@
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>24</v>
       </c>
@@ -2364,7 +2375,7 @@
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>24</v>
       </c>
@@ -2379,7 +2390,7 @@
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>24</v>
       </c>
@@ -2394,7 +2405,7 @@
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>24</v>
       </c>
@@ -2409,7 +2420,7 @@
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>24</v>
       </c>
@@ -2424,7 +2435,7 @@
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>24</v>
       </c>
@@ -2439,7 +2450,7 @@
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>24</v>
       </c>
@@ -2454,7 +2465,7 @@
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>24</v>
       </c>
@@ -2469,7 +2480,7 @@
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>24</v>
       </c>
@@ -2484,7 +2495,7 @@
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>24</v>
       </c>
@@ -2499,7 +2510,7 @@
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>24</v>
       </c>
@@ -2514,7 +2525,7 @@
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>24</v>
       </c>
@@ -2529,7 +2540,7 @@
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>24</v>
       </c>
@@ -2544,7 +2555,7 @@
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>24</v>
       </c>
@@ -2559,7 +2570,7 @@
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>24</v>
       </c>
@@ -2574,7 +2585,7 @@
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>24</v>
       </c>
@@ -2589,7 +2600,7 @@
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>24</v>
       </c>
@@ -2604,7 +2615,7 @@
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>24</v>
       </c>
@@ -2619,7 +2630,7 @@
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>24</v>
       </c>
@@ -2634,7 +2645,7 @@
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>24</v>
       </c>
@@ -2649,7 +2660,7 @@
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>24</v>
       </c>
@@ -2664,7 +2675,7 @@
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>24</v>
       </c>
@@ -2679,7 +2690,7 @@
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>24</v>
       </c>
@@ -2694,7 +2705,7 @@
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>24</v>
       </c>
@@ -2711,5 +2722,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>